<commit_message>
Added in struct prototype class for code minimisation
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\doom.js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D105A8B-1A52-40E4-A4F4-8FCD33594D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A96F915-9B56-45D3-A5F4-595422D0514B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C52A83A-498F-4034-B537-DF930780D4E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -792,7 +791,7 @@
   <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,16 +1845,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DBE406-FFD2-4258-BB4C-8397A96315C9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added in doomtype.h file
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\doom.js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0978E37F-28E8-40AD-9673-3617F350157B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F263F945-7D7A-4E9F-B5D1-9E944BB46F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C52A83A-498F-4034-B537-DF930780D4E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="132">
   <si>
     <t>am_map.c</t>
   </si>
@@ -791,7 +791,7 @@
   <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,11 +841,11 @@
       </c>
       <c r="G2">
         <f>SUMIFS(B2:B125,C2:C125,"Done")</f>
-        <v>598</v>
+        <v>664</v>
       </c>
       <c r="H2">
         <f>G2/F2*100</f>
-        <v>1.0944363103953147</v>
+        <v>1.2152269399707174</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,6 +1015,9 @@
       </c>
       <c r="B22">
         <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>